<commit_message>
hourly data refined (again)
</commit_message>
<xml_diff>
--- a/hourly datasets/cap_gen_year-1final.xlsx
+++ b/hourly datasets/cap_gen_year-1final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>100%&gt;gen/cap&gt;95%</t>
+          <t>10%&gt;gen/cap&gt;5%</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -490,679 +490,683 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>0.1644129276282225</v>
+        <v>0.1609937652266441</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>105%&gt;gen/cap&gt;100%</t>
+          <t>100%&gt;gen/cap&gt;95%</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.758508218996128e-05</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.0004803100634699367</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.5909276266103137</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.0649258012500506</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-0.0008838073890817962</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.0009989775534617192</v>
-      </c>
+        <v>0.06732675825338529</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>0.1644705127104125</v>
+        <v>0.2283205234800294</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110%&gt;gen/cap&gt;105%</t>
+          <t>105%&gt;gen/cap&gt;100%</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.004351211841010456</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0007048118004076447</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5.034528181572235</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.03206444660934276</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.002969803123422347</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.005732620558598565</v>
-      </c>
+        <v>0.07495267438501052</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>0.168764139469233</v>
+        <v>0.2359464396116546</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>115%&gt;gen/cap&gt;110%</t>
+          <t>110%&gt;gen/cap&gt;105%</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.01389885822959776</v>
+        <v>0.07031837262577524</v>
       </c>
       <c r="C5" t="n">
-        <v>0.001239881119939165</v>
+        <v>0.008301928843133622</v>
       </c>
       <c r="D5" t="n">
-        <v>11.54399051229067</v>
+        <v>-2898659457611.042</v>
       </c>
       <c r="E5" t="n">
-        <v>0.06990619334157348</v>
+        <v>0.06746850419104353</v>
       </c>
       <c r="F5" t="n">
-        <v>0.01146873069748544</v>
+        <v>0.05404243140926995</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01632898576171007</v>
+        <v>0.08659431384227945</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1783117858578203</v>
+        <v>0.2313121378524193</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>120%&gt;gen/cap&gt;115%</t>
+          <t>115%&gt;gen/cap&gt;110%</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.02543143238483607</v>
+        <v>0.0256679353092471</v>
       </c>
       <c r="C6" t="n">
-        <v>0.002755329223554764</v>
+        <v>0.004575382974968281</v>
       </c>
       <c r="D6" t="n">
-        <v>11.27388591042044</v>
+        <v>2.863724429748117</v>
       </c>
       <c r="E6" t="n">
-        <v>0.08769715160153979</v>
+        <v>0.07841388265548134</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02003107515514821</v>
+        <v>0.01669737712673798</v>
       </c>
       <c r="G6" t="n">
-        <v>0.03083178961452394</v>
+        <v>0.03463849349175589</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1898443600130586</v>
+        <v>0.1866617005358912</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>125%&gt;gen/cap&gt;120%</t>
+          <t>120%&gt;gen/cap&gt;115%</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.03691116647149409</v>
+        <v>0.01771203847967302</v>
       </c>
       <c r="C7" t="n">
-        <v>0.003659523230918313</v>
+        <v>0.002312714157955482</v>
       </c>
       <c r="D7" t="n">
-        <v>9.71775117415466</v>
+        <v>1.732859824749732</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0007549217411945617</v>
+        <v>0.05534163729948974</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02973861902010179</v>
+        <v>0.01317595815273482</v>
       </c>
       <c r="G7" t="n">
-        <v>0.04408371392288638</v>
+        <v>0.02224811880661143</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2013240940997166</v>
+        <v>0.1787058037063171</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>130%&gt;gen/cap&gt;125%</t>
+          <t>125%&gt;gen/cap&gt;120%</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.06365440046894059</v>
+        <v>0.01017962835927406</v>
       </c>
       <c r="C8" t="n">
-        <v>0.008745984312425755</v>
+        <v>0.001382291709391501</v>
       </c>
       <c r="D8" t="n">
-        <v>9.546819366059417</v>
+        <v>0.7394120925014661</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04443764656714787</v>
+        <v>0.05506278969102659</v>
       </c>
       <c r="F8" t="n">
-        <v>0.04651255294817385</v>
+        <v>0.007468783524116581</v>
       </c>
       <c r="G8" t="n">
-        <v>0.08079624798970733</v>
+        <v>0.0128904731944318</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2280673280971631</v>
+        <v>0.1711733935859182</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>135%&gt;gen/cap&gt;130%</t>
+          <t>130%&gt;gen/cap&gt;125%</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.07672014762727902</v>
+        <v>0.007078955541027616</v>
       </c>
       <c r="C9" t="n">
-        <v>0.004438300818557752</v>
+        <v>0.001339058309943384</v>
       </c>
       <c r="D9" t="n">
-        <v>14.73266693100093</v>
+        <v>0.2578219859705039</v>
       </c>
       <c r="E9" t="n">
-        <v>0.01512186483374011</v>
+        <v>0.03329880170089298</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06802122078768624</v>
+        <v>0.004453323458616759</v>
       </c>
       <c r="G9" t="n">
-        <v>0.08541907446687183</v>
+        <v>0.009704587623438628</v>
       </c>
       <c r="H9" t="n">
-        <v>0.2411330752555016</v>
+        <v>0.1680727207676717</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20%&gt;gen/cap</t>
+          <t>135%&gt;gen/cap&gt;130%</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.1644129276282225</v>
+        <v>0.001347583734443785</v>
       </c>
       <c r="C10" t="n">
-        <v>0.002243874384109128</v>
+        <v>0.0004606859041834599</v>
       </c>
       <c r="D10" t="n">
-        <v>-191.7192430660797</v>
+        <v>0.06010202711669116</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.03486214024434322</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.1688110982738554</v>
+        <v>0.0004442649395541191</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.1600147569825897</v>
+        <v>0.002250902529333486</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.1623413489610879</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>25%&gt;gen/cap&gt;20%</t>
+          <t>15%&gt;gen/cap&gt;10%</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.1180953598053943</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.00230108846641554</v>
-      </c>
-      <c r="D11" t="n">
-        <v>-62.31998862253953</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>-0.1226056689305536</v>
-      </c>
-      <c r="G11" t="n">
-        <v>-0.1135850506802349</v>
-      </c>
+        <v>0.02342172758121825</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
-        <v>0.04631756782282828</v>
+        <v>0.1844154928078623</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>30%&gt;gen/cap&gt;25%</t>
+          <t>20%&gt;gen/cap&gt;15%</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.1129802957303966</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.002288081786349923</v>
-      </c>
-      <c r="D12" t="n">
-        <v>-54.07475025172925</v>
-      </c>
-      <c r="E12" t="n">
-        <v>2.093981562406875e-133</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-0.117465112047717</v>
-      </c>
-      <c r="G12" t="n">
-        <v>-0.1084954794130763</v>
-      </c>
+        <v>0.03763462393322742</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
-        <v>0.0514326318978259</v>
+        <v>0.1986283891598715</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>35%&gt;gen/cap&gt;30%</t>
+          <t>25%&gt;gen/cap&gt;20%</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.1061821189147043</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.00228513270710968</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-40.11540882328785</v>
-      </c>
-      <c r="E13" t="n">
-        <v>2.033919606352092e-89</v>
-      </c>
-      <c r="F13" t="n">
-        <v>-0.1106611550874712</v>
-      </c>
-      <c r="G13" t="n">
-        <v>-0.1017030827419374</v>
-      </c>
+        <v>0.04438888331551254</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
-        <v>0.05823080871351823</v>
+        <v>0.2053826485421567</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>40%&gt;gen/cap&gt;35%</t>
+          <t>30%&gt;gen/cap&gt;25%</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.1022858159095502</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.002277654074857105</v>
-      </c>
-      <c r="D14" t="n">
-        <v>-33.59307620066063</v>
-      </c>
-      <c r="E14" t="n">
-        <v>3.057583442135537e-52</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-0.1067501941241174</v>
-      </c>
-      <c r="G14" t="n">
-        <v>-0.09782143769498301</v>
-      </c>
+        <v>0.04944361483145905</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
-        <v>0.06212711171867236</v>
+        <v>0.2104373800581031</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>45%&gt;gen/cap&gt;40%</t>
+          <t>35%&gt;gen/cap&gt;30%</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.1010375239842642</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.00227718802861228</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-29.99117738407764</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.01290549744408518</v>
-      </c>
-      <c r="F15" t="n">
-        <v>-0.1055009902273536</v>
-      </c>
-      <c r="G15" t="n">
-        <v>-0.09657405774117486</v>
-      </c>
+        <v>0.05401530431502669</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
-        <v>0.0633754036439583</v>
+        <v>0.2150090695416708</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>50%&gt;gen/cap&gt;45%</t>
+          <t>40%&gt;gen/cap&gt;35%</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.09780029536251636</v>
+        <v>0.05779928885048211</v>
       </c>
       <c r="C16" t="n">
-        <v>0.002250353968463219</v>
+        <v>0.007403461896217422</v>
       </c>
       <c r="D16" t="n">
-        <v>-22.60803989326072</v>
+        <v>11.85849268626988</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0005965398823098759</v>
+        <v>0.05223502247494265</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.1022111663676216</v>
+        <v>0.04327622260331647</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.09338942435741114</v>
+        <v>0.07232235509764777</v>
       </c>
       <c r="H16" t="n">
-        <v>0.06661263226570618</v>
+        <v>0.2187930540771262</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>55%&gt;gen/cap&gt;50%</t>
+          <t>45%&gt;gen/cap&gt;40%</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.09598170016901199</v>
+        <v>0.0607907447738734</v>
       </c>
       <c r="C17" t="n">
-        <v>0.002258795280635513</v>
+        <v>0.007236831726647693</v>
       </c>
       <c r="D17" t="n">
-        <v>-19.25562965828096</v>
+        <v>12.23210076616483</v>
       </c>
       <c r="E17" t="n">
-        <v>0.03200901312615248</v>
+        <v>0.04936085916821359</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.1004091157989204</v>
+        <v>0.04659588638668243</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.09155428453910362</v>
+        <v>0.07498560316106433</v>
       </c>
       <c r="H17" t="n">
-        <v>0.06843122745921056</v>
+        <v>0.2217845100005175</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>60%&gt;gen/cap&gt;55%</t>
+          <t>5%&gt;gen/cap</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.09661350390589202</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.002276968781796699</v>
-      </c>
-      <c r="D18" t="n">
-        <v>-20.01972592817874</v>
-      </c>
-      <c r="E18" t="n">
-        <v>4.355144981995015e-17</v>
-      </c>
-      <c r="F18" t="n">
-        <v>-0.101076539295671</v>
-      </c>
-      <c r="G18" t="n">
-        <v>-0.092150468516113</v>
-      </c>
+        <v>-0.1609937652266441</v>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
-        <v>0.06779942372233053</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>65%&gt;gen/cap&gt;60%</t>
+          <t>50%&gt;gen/cap&gt;45%</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.09542460816127066</v>
+        <v>0.06317991434890674</v>
       </c>
       <c r="C19" t="n">
-        <v>0.002272279519674028</v>
+        <v>0.007251546407040833</v>
       </c>
       <c r="D19" t="n">
-        <v>-17.42370052049663</v>
+        <v>2205657588155.395</v>
       </c>
       <c r="E19" t="n">
-        <v>0.05676788889894999</v>
+        <v>0.05355010983478414</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.09987845253019281</v>
+        <v>0.04895466508766864</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.0909707637923485</v>
+        <v>0.07740516361014484</v>
       </c>
       <c r="H19" t="n">
-        <v>0.06898831946695189</v>
+        <v>0.2241736795755508</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>70%&gt;gen/cap&gt;65%</t>
+          <t>55%&gt;gen/cap&gt;50%</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.09413499564909475</v>
+        <v>0.06333486923089782</v>
       </c>
       <c r="C20" t="n">
-        <v>0.002270188462699432</v>
+        <v>0.007470459942775563</v>
       </c>
       <c r="D20" t="n">
-        <v>-14.85734482035729</v>
+        <v>-2146861501808.214</v>
       </c>
       <c r="E20" t="n">
-        <v>4.634251236031497e-08</v>
+        <v>0.05701375089264056</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.09858474152728373</v>
+        <v>0.04867969240930516</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.08968524977090579</v>
+        <v>0.07799004605249028</v>
       </c>
       <c r="H20" t="n">
-        <v>0.07027793197912779</v>
+        <v>0.2243286344575419</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>75%&gt;gen/cap&gt;70%</t>
+          <t>60%&gt;gen/cap&gt;55%</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.09275783981102494</v>
+        <v>0.06311178390145847</v>
       </c>
       <c r="C21" t="n">
-        <v>0.002272551609604951</v>
+        <v>0.007264729977244719</v>
       </c>
       <c r="D21" t="n">
-        <v>-11.70854067857449</v>
+        <v>12.33083495560344</v>
       </c>
       <c r="E21" t="n">
-        <v>0.04741532826272409</v>
+        <v>0.05973643227610392</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.09721221731561254</v>
+        <v>0.04886095184582429</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.08830346230643732</v>
+        <v>0.07736261595709273</v>
       </c>
       <c r="H21" t="n">
-        <v>0.07165508781719761</v>
+        <v>0.2241055491281026</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>80%&gt;gen/cap&gt;75%</t>
+          <t>65%&gt;gen/cap&gt;60%</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.09225948159139878</v>
+        <v>0.06352882323557643</v>
       </c>
       <c r="C22" t="n">
-        <v>0.002273501726105746</v>
+        <v>0.007258909351113647</v>
       </c>
       <c r="D22" t="n">
-        <v>-10.5313126399131</v>
+        <v>12.34414641217973</v>
       </c>
       <c r="E22" t="n">
-        <v>0.1409026714340376</v>
+        <v>0.06243387354347495</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.09671572127399256</v>
+        <v>0.04928659607536647</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.08780324190880501</v>
+        <v>0.07777105039578659</v>
       </c>
       <c r="H22" t="n">
-        <v>0.07215344603682376</v>
+        <v>0.2245225884622205</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>85%&gt;gen/cap&gt;80%</t>
+          <t>70%&gt;gen/cap&gt;65%</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.09222666751552397</v>
+        <v>0.06563676626897748</v>
       </c>
       <c r="C23" t="n">
-        <v>0.002269642164071812</v>
+        <v>0.007439969666634025</v>
       </c>
       <c r="D23" t="n">
-        <v>-9.835732186460994</v>
+        <v>12.76314161521639</v>
       </c>
       <c r="E23" t="n">
-        <v>0.001284690234720559</v>
+        <v>0.0575798220498769</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.09667534256942106</v>
+        <v>0.05104184199701441</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.08777799246162687</v>
+        <v>0.08023169054094062</v>
       </c>
       <c r="H23" t="n">
-        <v>0.07218626011269857</v>
+        <v>0.2266305314956216</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>90%&gt;gen/cap&gt;85%</t>
+          <t>75%&gt;gen/cap&gt;70%</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.09121385252631713</v>
+        <v>0.06632239330511167</v>
       </c>
       <c r="C24" t="n">
-        <v>0.002261988119252753</v>
+        <v>0.007261747254362975</v>
       </c>
       <c r="D24" t="n">
-        <v>-7.612359177293491</v>
+        <v>12.89644886104007</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0752364297671903</v>
+        <v>0.06136057187355696</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.09564752591302747</v>
+        <v>0.05207835314917655</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.08678017913960677</v>
+        <v>0.0805664334610466</v>
       </c>
       <c r="H24" t="n">
-        <v>0.07319907510190542</v>
+        <v>0.2273161585317558</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>95%&gt;gen/cap&gt;90%</t>
+          <t>80%&gt;gen/cap&gt;75%</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.09117940612506044</v>
+        <v>0.06776715574512451</v>
       </c>
       <c r="C25" t="n">
-        <v>0.002243692375172767</v>
+        <v>0.007482761128377513</v>
       </c>
       <c r="D25" t="n">
-        <v>-7.227941587541884</v>
+        <v>15690696889049.63</v>
       </c>
       <c r="E25" t="n">
-        <v>0.06224714065280199</v>
+        <v>0.07174640948675752</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.09557722043539583</v>
+        <v>0.05309059309092674</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.08678159181472506</v>
+        <v>0.08244371839932242</v>
       </c>
       <c r="H25" t="n">
-        <v>0.07323352150316211</v>
+        <v>0.2287609209717686</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>85%&gt;gen/cap&gt;80%</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.06746573575592232</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.007389980821796724</v>
+      </c>
+      <c r="D26" t="n">
+        <v>12.60653218430758</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.06847121578709091</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.05297183633920472</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.08195963517263999</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.2284595009825664</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>90%&gt;gen/cap&gt;85%</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.06681108101383898</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.007719688318505421</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-2977424450330.677</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.06222326196274704</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.05167070774314321</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.08195145428453461</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.2278048462404831</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>95%&gt;gen/cap&gt;90%</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.06778880662172586</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.007550059691334927</v>
+      </c>
+      <c r="D28" t="n">
+        <v>12.43989950791204</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.08681465862014252</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.05298058092188872</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.08259703232156294</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.22878257184837</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>gen/cap&gt;135%</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>0.08841575640935871</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.007104862305268717</v>
-      </c>
-      <c r="D26" t="n">
-        <v>23.48487550540731</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.0006076735914554184</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.07449045326680986</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.1023410595519076</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.2528286840375812</v>
+      <c r="B29" t="n">
+        <v>0.01051821696571737</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.001249550696893102</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.624653633552927</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.01020129227988134</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.008064612613370022</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.01297182131806454</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.1715119821923615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>